<commit_message>
Generalized number  and date format (#289)
* Add a generalized datetime parser

* Add generalized number format

* Remove re import

* Add blank lines for linting

* Use different string type

* Fix capital letter in General

* Handle code with no spaces

* Add new tests

* Remove print statement

* Remove extra tab
</commit_message>
<xml_diff>
--- a/data/special/preserve-formatting.xlsx
+++ b/data/special/preserve-formatting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">empty</t>
   </si>
@@ -31,13 +31,13 @@
     <t xml:space="preserve">0.00</t>
   </si>
   <si>
-    <t xml:space="preserve">#,##0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#,##0.00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">#,###.00</t>
+    <t xml:space="preserve">0.0000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0000#</t>
   </si>
   <si>
     <t xml:space="preserve">m/d/yy</t>
@@ -47,28 +47,37 @@
   </si>
   <si>
     <t xml:space="preserve">mm/dd/yy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmddyy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mmddyyam/pmdd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="9">
+  <numFmts count="11">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="#,##0"/>
-    <numFmt numFmtId="168" formatCode="#,##0.00"/>
-    <numFmt numFmtId="169" formatCode="#,###.00"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0000#"/>
     <numFmt numFmtId="170" formatCode="M/D/YY"/>
     <numFmt numFmtId="171" formatCode="D\-MMM"/>
     <numFmt numFmtId="172" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="173" formatCode="MMDDYY"/>
+    <numFmt numFmtId="174" formatCode="MMDDYYAM/PMDD"/>
   </numFmts>
   <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -128,7 +137,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -169,14 +178,22 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -186,16 +203,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="1" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="1" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.83"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1022" min="12" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -226,6 +244,12 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
@@ -250,6 +274,12 @@
         <v>51276</v>
       </c>
       <c r="I2" s="9" t="n">
+        <v>51276</v>
+      </c>
+      <c r="J2" s="10" t="n">
+        <v>51276</v>
+      </c>
+      <c r="K2" s="11" t="n">
         <v>51276</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix excel number @ (#345)
* Handle @ symbol in xlsx number_format

* Add test
</commit_message>
<xml_diff>
--- a/data/special/preserve-formatting.xlsx
+++ b/data/special/preserve-formatting.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">empty</t>
   </si>
@@ -53,24 +53,28 @@
   </si>
   <si>
     <t xml:space="preserve">mmddyyam/pmdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at_symbol</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.0000#"/>
-    <numFmt numFmtId="170" formatCode="M/D/YY"/>
-    <numFmt numFmtId="171" formatCode="D\-MMM"/>
-    <numFmt numFmtId="172" formatCode="MM/DD/YY"/>
-    <numFmt numFmtId="173" formatCode="MMDDYY"/>
-    <numFmt numFmtId="174" formatCode="MMDDYYAM/PMDD"/>
+    <numFmt numFmtId="170" formatCode="m/d/yy"/>
+    <numFmt numFmtId="171" formatCode="d\-mmm"/>
+    <numFmt numFmtId="172" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="173" formatCode="mmddyy"/>
+    <numFmt numFmtId="174" formatCode="mmddyyAM/PMdd"/>
+    <numFmt numFmtId="175" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -137,7 +141,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +188,10 @@
     </xf>
     <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -199,14 +207,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="L2" activeCellId="0" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -250,6 +258,9 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
@@ -281,6 +292,9 @@
       </c>
       <c r="K2" s="11" t="n">
         <v>51276</v>
+      </c>
+      <c r="L2" s="12" t="n">
+        <v>259.153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>